<commit_message>
fix bug, archive, version
</commit_message>
<xml_diff>
--- a/2048_Rbu/Data/Service.xlsx
+++ b/2048_Rbu/Data/Service.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Files\Work\Project\2020\2048_РБУ\PC\2048_RBU\2048_Rbu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E027A8B-3083-4959-B688-5E820CE443E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB6FD4C-443C-49D0-A746-65DB6CF97AAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{6A7DC8BC-89CE-448E-885C-39A392A11F89}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{6A7DC8BC-89CE-448E-885C-39A392A11F89}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Oбъект</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>192.168.100.90</t>
+  </si>
+  <si>
+    <t>CheckVersion</t>
   </si>
 </sst>
 </file>
@@ -279,11 +282,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873DFC9-5EB5-42AA-B27E-8D7A5DD4C0B0}">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +848,10 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="5"/>
@@ -865,11 +868,19 @@
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>43</v>
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new, fix bug
</commit_message>
<xml_diff>
--- a/2048_Rbu/Data/Service.xlsx
+++ b/2048_Rbu/Data/Service.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Files\Work\Project\2020\2048_РБУ\PC\2048_RBU\2048_Rbu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C337CCDC-7526-4749-BE97-1F62814560CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BA5D5-C615-4950-8830-EAF25BB0FCBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6A7DC8BC-89CE-448E-885C-39A392A11F89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A7DC8BC-89CE-448E-885C-39A392A11F89}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Oбъект</t>
   </si>
@@ -154,14 +154,17 @@
     <t>Cipher</t>
   </si>
   <si>
-    <t>Программа управления
+    <t>CheckVersion</t>
+  </si>
+  <si>
+    <t>192.168.100.90</t>
+  </si>
+  <si>
+    <t>Программа управления 
 растворо-бетонным узлом</t>
   </si>
   <si>
-    <t>192.168.100.90</t>
-  </si>
-  <si>
-    <t>CheckVersion</t>
+    <t>localhost</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -685,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -852,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
@@ -869,7 +872,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
[Redesign_RBU] - Changed "localhost" to IP to run
</commit_message>
<xml_diff>
--- a/2048_Rbu/Data/Service.xlsx
+++ b/2048_Rbu/Data/Service.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Files\Work\Project\2020\2048_РБУ\PC\2048_RBU\2048_Rbu\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MINE\Darvas\Git\ASU-Techno_2048_RBU\2048_Rbu\2048_Rbu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BA5D5-C615-4950-8830-EAF25BB0FCBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8593AD2B-654F-431B-B852-01D28B5F9DEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A7DC8BC-89CE-448E-885C-39A392A11F89}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 растворо-бетонным узлом</t>
   </si>
   <si>
-    <t>localhost</t>
+    <t>192.168.100.70</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>